<commit_message>
End of implementation (ou presque...)
</commit_message>
<xml_diff>
--- a/bigLow.xlsx
+++ b/bigLow.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\teraetu\homeetu\c\p1608557\Mes documents\NetBeansProjects\MASproject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\i3mainz\Desktop\Projet L3\MASproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -919,8 +919,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -937,17 +937,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>bigLow!$B$1:$CW$2</c:f>
@@ -1565,7 +1562,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1575,12 +1571,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="117598344"/>
-        <c:axId val="117599520"/>
-      </c:lineChart>
+        <c:axId val="147476904"/>
+        <c:axId val="147477688"/>
+      </c:areaChart>
       <c:catAx>
-        <c:axId val="117598344"/>
+        <c:axId val="147476904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1623,7 +1618,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117599520"/>
+        <c:crossAx val="147477688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1631,7 +1626,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117599520"/>
+        <c:axId val="147477688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1682,9 +1677,864 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117598344"/>
+        <c:crossAx val="147476904"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>bigLow!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>nbIterations</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>bigLow!$B$1:$CW$2</c:f>
+              <c:strCache>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63.0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66.0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67.0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69.0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>71.0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73.0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>74.0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>75.0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>78.0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>79.0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>81.0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>82.0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>83.0</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>84.0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>85.0</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>86.0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>88.0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>89.0</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>92.0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>93.0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>94.0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>95.0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>96.0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>97.0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>98.0</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>99.0</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>100.0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>bigLow!$B$3:$CW$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>766452</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1146043</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>502434</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>433061</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>379054</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>229964</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>361323</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>241904</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>172515</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>171628</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>161601</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>139617</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>133063</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>139056</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41291</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>120807</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>104663</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>59214</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>91994</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>35403</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>76993</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>39834</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>88615</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>66892</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>86165</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>73876</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43495</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>35742</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>72427</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>53877</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>26840</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>39526</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>56827</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>38114</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>37748</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>40808</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>43983</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>73288</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>35837</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>49433</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>25818</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>39673</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>56291</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>56381</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>37916</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>51375</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>48880</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>43013</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>27173</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>27764</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>40396</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>39939</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>35698</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>24187</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>18877</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>30440</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>24408</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>40095</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>29000</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>25495</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>31094</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>25649</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>34420</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>20641</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>28410</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>12701</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>32930</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>23765</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>24670</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>25971</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>22168</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>24137</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>11352</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>29722</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>27026</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>23256</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>25655</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>20935</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>14856</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>17644</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>22307</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>14889</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>15512</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>12193</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>23650</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>10964</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>27648</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>13445</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>16512</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>17380</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>11637</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>12001</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>21470</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>17162</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>16598</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>12583</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>11958</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>22840</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>15711</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>19813</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="193105184"/>
+        <c:axId val="193107144"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="193105184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="193107144"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="193107144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="193105184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1771,7 +2621,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2314,6 +3720,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>61912</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2587,8 +4023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CW3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CF13" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:CW3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>